<commit_message>
added no.ID and Noise
</commit_message>
<xml_diff>
--- a/BatSpecies.xlsx
+++ b/BatSpecies.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/monae/Documents/DataLab/bats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rutte\OneDrive\Documents\DataLab\Bats\bats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CD0C729-0492-8145-A2BD-ED539EA98B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DA5753-6ACD-4AC7-8CF0-232C095208CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11120" yWindow="500" windowWidth="17300" windowHeight="16280" xr2:uid="{1A73A8D7-A6DF-E741-A3BB-D39F1158950E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{1A73A8D7-A6DF-E741-A3BB-D39F1158950E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>AUTO.ID</t>
   </si>
@@ -170,6 +170,12 @@
   </si>
   <si>
     <t>Perimyotis subflavus</t>
+  </si>
+  <si>
+    <t>no.ID</t>
+  </si>
+  <si>
+    <t>Noise</t>
   </si>
 </sst>
 </file>
@@ -521,15 +527,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9A9942D-0EC2-A442-A77B-D2FE04359C5C}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -551,7 +557,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -562,7 +568,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -573,7 +579,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -584,7 +590,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -595,7 +601,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -606,7 +612,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -617,7 +623,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -628,7 +634,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -639,7 +645,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -650,7 +656,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -661,7 +667,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -672,7 +678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -683,7 +689,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -692,6 +698,28 @@
       </c>
       <c r="C15" t="s">
         <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>